<commit_message>
More features in concept
</commit_message>
<xml_diff>
--- a/Game concept.xlsx
+++ b/Game concept.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>Must have features</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>dialogue</t>
+  </si>
+  <si>
+    <t>healing potion</t>
   </si>
   <si>
     <t>hub world (fifth levle)</t>
@@ -412,19 +415,22 @@
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B10" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="C10" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>36</v>
@@ -436,58 +442,58 @@
     <row r="12">
       <c r="A12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>4</v>

</xml_diff>